<commit_message>
Update notes, log, and create directories in an unsuccessful attempt to properly install pyopencl on Windows 10
</commit_message>
<xml_diff>
--- a/Exercises/log/IH_timecard.xlsx
+++ b/Exercises/log/IH_timecard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Viz2\python_anaconda3\UCB ABC\git_clones\LLS_Pipeline\Exercises\log\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86AD453B-B6A3-4F5A-A550-03FF0BF2CD01}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{119DB0C8-7CC0-42C2-9383-76D6A0853764}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="12330" xr2:uid="{5BC6551A-4641-43C0-88F7-21ABDBFD94F2}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>IMG PROCESSING PIPELINE - TIMECARD FOR IRA HORECKA</t>
   </si>
@@ -64,6 +64,18 @@
   </si>
   <si>
     <t>Complete Matthew Rocklin's tutorial on using GPUs for large numpy array computation</t>
+  </si>
+  <si>
+    <t>Work with numba on Windows 10</t>
+  </si>
+  <si>
+    <t>Try to install pyopencl without import error</t>
+  </si>
+  <si>
+    <t>Afterwards, attempt to use llspy and spimagine, which both have opencl dependencies</t>
+  </si>
+  <si>
+    <t>Cannot install pyopencl without import error - give up for now and look to working with Linux</t>
   </si>
 </sst>
 </file>
@@ -425,10 +437,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0198F2CD-E31C-43FB-ACFA-EF7ACCB6D806}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -492,6 +504,29 @@
         <v>10</v>
       </c>
     </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>43866</v>
+      </c>
+      <c r="B14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
add Modules directory && update README
</commit_message>
<xml_diff>
--- a/Exercises/log/IH_timecard.xlsx
+++ b/Exercises/log/IH_timecard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Viz2\python_anaconda3\UCB ABC\git_clones\LLS_Pipeline\Exercises\log\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48782061-B1ED-4DC1-8A47-AD8C641D7C43}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CECC55E2-D87A-4A6E-B26B-C2ECC4A4C56D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4500" yWindow="6555" windowWidth="24000" windowHeight="12330" xr2:uid="{5BC6551A-4641-43C0-88F7-21ABDBFD94F2}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>IMG PROCESSING PIPELINE - TIMECARD FOR IRA HORECKA</t>
   </si>
@@ -88,6 +88,21 @@
   </si>
   <si>
     <t>Installed CUDA Toolkit 10.1, pip install cupy-cuda101 successfully</t>
+  </si>
+  <si>
+    <t>Create script to parallelize writing to Zarr files (Viz2)</t>
+  </si>
+  <si>
+    <t>Use dask distributed rather than multirprocessing to accomplish this task</t>
+  </si>
+  <si>
+    <t>Curate scripts for parallel writing to Zarr files</t>
+  </si>
+  <si>
+    <t>Create simple script to read Zarr files to either Zarr intermediate or dask</t>
+  </si>
+  <si>
+    <t>Curate repository and update README</t>
   </si>
 </sst>
 </file>
@@ -449,13 +464,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0198F2CD-E31C-43FB-ACFA-EF7ACCB6D806}">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -560,6 +578,37 @@
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>43873</v>
+      </c>
+      <c r="B24" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
+        <v>43874</v>
+      </c>
+      <c r="B27" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
clone napari, naparimovie for mod
</commit_message>
<xml_diff>
--- a/Exercises/log/IH_timecard.xlsx
+++ b/Exercises/log/IH_timecard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Viz2\python_anaconda3\UCB ABC\git_clones\LLS_Pipeline\Exercises\log\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CECC55E2-D87A-4A6E-B26B-C2ECC4A4C56D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B329F2CE-80D0-4AF8-9628-E4E9D81FAB5D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4500" yWindow="6555" windowWidth="24000" windowHeight="12330" xr2:uid="{5BC6551A-4641-43C0-88F7-21ABDBFD94F2}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>IMG PROCESSING PIPELINE - TIMECARD FOR IRA HORECKA</t>
   </si>
@@ -103,6 +103,12 @@
   </si>
   <si>
     <t>Curate repository and update README</t>
+  </si>
+  <si>
+    <t>Refactor write and read zarr file code</t>
+  </si>
+  <si>
+    <t>Plan for incorporating napari pipeline with napari movie</t>
   </si>
 </sst>
 </file>
@@ -464,10 +470,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0198F2CD-E31C-43FB-ACFA-EF7ACCB6D806}">
-  <dimension ref="A1:B29"/>
+  <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -611,6 +617,19 @@
         <v>23</v>
       </c>
     </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
+        <v>43875</v>
+      </c>
+      <c r="B31" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>